<commit_message>
Refactorizo clase DetalleFSR para agregar clean code y oculto el boton Seguimiento de Servicios de la clase DetalleFSR
</commit_message>
<xml_diff>
--- a/INOLAB_OC/Docs/28392.xlsx
+++ b/INOLAB_OC/Docs/28392.xlsx
@@ -6,13 +6,13 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R67705385d0544002"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R3b506ba469dd4fa1"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <x:si>
     <x:t>IdFSR</x:t>
   </x:si>
@@ -59,9 +59,6 @@
     <x:t>Ingeniero</x:t>
   </x:si>
   <x:si>
-    <x:t>IdIngeniero</x:t>
-  </x:si>
-  <x:si>
     <x:t>mailIng</x:t>
   </x:si>
   <x:si>
@@ -216,117 +213,6 @@
   </x:si>
   <x:si>
     <x:t>NombreCliente</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2906</x:t>
-  </x:si>
-  <x:si>
-    <x:t>28392</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Neolpharma</x:t>
-  </x:si>
-  <x:si>
-    <x:t>COLTROL FISICOQUIMICO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Blvd. de los Ferrocarriles, Col. Industrial Vallejo, C.P. 02300</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5548553967</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Azcapotzalco, </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Emiliano Vergara</x:t>
-  </x:si>
-  <x:si>
-    <x:t>emiliano.vergara@neolpharma.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Contrato Classic</x:t>
-  </x:si>
-  <x:si>
-    <x:t>N/A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mant. Prev.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MANTTO. PREV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Lebni Torres Colin</x:t>
-  </x:si>
-  <x:si>
-    <x:t>46</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lebnitorres@inolab.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2022-06-10 13:40:09.000</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2022-06-15</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Friabilizador 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pharmatron</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FT20</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1305205</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EA-80-Q140</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Asignado</x:t>
-  </x:si>
-  <x:si>
-    <x:t>740</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Miercoles</x:t>
-  </x:si>
-  <x:si>
-    <x:t>09:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4734</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sin Confirmar</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Dinorath</x:t>
-  </x:si>
-  <x:si>
-    <x:t>dinorathchamu@inolab.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>No</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12102</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -657,7 +543,7 @@
 
 <file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:BP2"/>
+  <x:dimension ref="A1:BO1"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -865,140 +751,6 @@
       <x:c r="BO1" t="s">
         <x:v>66</x:v>
       </x:c>
-      <x:c r="BP1" t="s">
-        <x:v>67</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2">
-      <x:c r="A2" t="s">
-        <x:v>68</x:v>
-      </x:c>
-      <x:c r="B2" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="C2" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="D2" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="E2" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="F2" t="s">
-        <x:v>73</x:v>
-      </x:c>
-      <x:c r="G2" t="s">
-        <x:v>74</x:v>
-      </x:c>
-      <x:c r="H2" t="s">
-        <x:v>75</x:v>
-      </x:c>
-      <x:c r="I2" t="s">
-        <x:v>75</x:v>
-      </x:c>
-      <x:c r="J2" t="s">
-        <x:v>76</x:v>
-      </x:c>
-      <x:c r="K2" t="s">
-        <x:v>77</x:v>
-      </x:c>
-      <x:c r="L2" t="s">
-        <x:v>78</x:v>
-      </x:c>
-      <x:c r="M2" t="s">
-        <x:v>79</x:v>
-      </x:c>
-      <x:c r="N2" t="s">
-        <x:v>80</x:v>
-      </x:c>
-      <x:c r="O2" t="s">
-        <x:v>81</x:v>
-      </x:c>
-      <x:c r="P2" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="Q2" t="s">
-        <x:v>83</x:v>
-      </x:c>
-      <x:c r="R2" t="s">
-        <x:v>84</x:v>
-      </x:c>
-      <x:c r="S2" t="s">
-        <x:v>85</x:v>
-      </x:c>
-      <x:c r="T2" t="s">
-        <x:v>86</x:v>
-      </x:c>
-      <x:c r="U2" t="s">
-        <x:v>87</x:v>
-      </x:c>
-      <x:c r="V2" t="s">
-        <x:v>88</x:v>
-      </x:c>
-      <x:c r="W2" t="s">
-        <x:v>89</x:v>
-      </x:c>
-      <x:c r="X2" t="s">
-        <x:v>90</x:v>
-      </x:c>
-      <x:c r="Y2" t="s">
-        <x:v>91</x:v>
-      </x:c>
-      <x:c r="Z2" t="s">
-        <x:v>92</x:v>
-      </x:c>
-      <x:c r="AB2" t="s">
-        <x:v>93</x:v>
-      </x:c>
-      <x:c r="AE2" t="s">
-        <x:v>94</x:v>
-      </x:c>
-      <x:c r="AF2" t="s">
-        <x:v>78</x:v>
-      </x:c>
-      <x:c r="AG2" t="s">
-        <x:v>95</x:v>
-      </x:c>
-      <x:c r="AJ2" t="s">
-        <x:v>96</x:v>
-      </x:c>
-      <x:c r="AK2" t="s">
-        <x:v>97</x:v>
-      </x:c>
-      <x:c r="AL2" t="s">
-        <x:v>98</x:v>
-      </x:c>
-      <x:c r="AM2" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="AN2" t="s">
-        <x:v>83</x:v>
-      </x:c>
-      <x:c r="AP2" t="s">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="AQ2" t="s">
-        <x:v>101</x:v>
-      </x:c>
-      <x:c r="AR2" t="s">
-        <x:v>102</x:v>
-      </x:c>
-      <x:c r="AW2" t="s">
-        <x:v>103</x:v>
-      </x:c>
-      <x:c r="BF2" t="s">
-        <x:v>101</x:v>
-      </x:c>
-      <x:c r="BG2" t="s">
-        <x:v>104</x:v>
-      </x:c>
-      <x:c r="BH2" t="s">
-        <x:v>103</x:v>
-      </x:c>
-      <x:c r="BK2" t="s">
-        <x:v>91</x:v>
-      </x:c>
     </x:row>
   </x:sheetData>
 </x:worksheet>

</xml_diff>